<commit_message>
Update to work with no video
</commit_message>
<xml_diff>
--- a/src/gold-miner-classic-origin-metadata-translate.xlsx
+++ b/src/gold-miner-classic-origin-metadata-translate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="456">
   <si>
     <t>English</t>
   </si>
@@ -1436,6 +1436,9 @@
   </si>
   <si>
     <t>Youtube URL (Android)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>APK's version code 
@@ -1529,7 +1532,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1562,6 +1565,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
@@ -4183,7 +4189,9 @@
       <c r="A8" t="s" s="3">
         <v>452</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" t="s" s="11">
+        <v>453</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -4252,11 +4260,11 @@
       <c r="BP8" s="2"/>
     </row>
     <row r="9" ht="49.55" customHeight="1">
-      <c r="A9" t="s" s="11">
-        <v>453</v>
+      <c r="A9" t="s" s="12">
+        <v>454</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>

</xml_diff>